<commit_message>
optimisation pesées en cours
</commit_message>
<xml_diff>
--- a/jauges.xlsx
+++ b/jauges.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>moyenne</t>
   </si>
@@ -35,10 +35,22 @@
     <t>E - C</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>ech</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Av</t>
+  </si>
+  <si>
+    <t>{-21000,-23208.92,20,0},     // J03 évolution valeurs en négatif. tester sur bornier</t>
+  </si>
+  <si>
+    <t>Tare</t>
+  </si>
+  <si>
+    <t>DHT22</t>
   </si>
 </sst>
 </file>
@@ -363,20 +375,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1">
-        <v>0</v>
+      <c r="C1" t="s">
+        <v>6</v>
       </c>
       <c r="E1">
         <v>2.331</v>
@@ -385,10 +400,10 @@
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>19</v>
       </c>
@@ -407,7 +422,7 @@
         <v>109204.63320463321</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>21</v>
       </c>
@@ -426,7 +441,7 @@
         <v>106727.58472758473</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>14</v>
       </c>
@@ -445,7 +460,7 @@
         <v>103286.14328614328</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>17</v>
       </c>
@@ -456,7 +471,7 @@
         <v>393888</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
+        <f>+E5-C5</f>
         <v>243290</v>
       </c>
       <c r="I5">
@@ -464,9 +479,118 @@
         <v>104371.51437151438</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G7" t="s">
-        <v>2</v>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <f t="shared" ref="G6:G8" si="1">+E6-C6</f>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f>G6/poids</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-21800</v>
+      </c>
+      <c r="E7" s="1">
+        <v>-75900</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>-54100</v>
+      </c>
+      <c r="I7">
+        <f>G7/poids</f>
+        <v>-23208.92320892321</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>-35751</v>
+      </c>
+      <c r="E8" s="1">
+        <v>-88863</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>-53112</v>
+      </c>
+      <c r="I8">
+        <f>G8/poids</f>
+        <v>-22785.070785070784</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1">
+        <v>-28026</v>
+      </c>
+      <c r="E9" s="1">
+        <v>-81617</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ref="G9" si="2">+E9-C9</f>
+        <v>-53591</v>
+      </c>
+      <c r="I9">
+        <f>G9/poids</f>
+        <v>-22990.56199056199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="J10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>-21000</v>
+      </c>
+      <c r="B14">
+        <v>-75826</v>
+      </c>
+      <c r="D14">
+        <f>B14-A14</f>
+        <v>-54826</v>
+      </c>
+      <c r="F14">
+        <f>D14*-1</f>
+        <v>54826</v>
+      </c>
+      <c r="H14">
+        <f>D14/I7</f>
+        <v>2.3622810720887246</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <f>F14/I7</f>
+        <v>-2.3622810720887246</v>
+      </c>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>